<commit_message>
added assets and queues. Transactions are now made by retrieving queue items from queue on Orchestrator.
</commit_message>
<xml_diff>
--- a/Project2/Orders.xlsx
+++ b/Project2/Orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3278B-5F09-41FC-B500-4D8D54A77457}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BE94B-C16F-461F-92D1-EE6F9204A9D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Product</t>
   </si>
@@ -91,7 +91,13 @@
     <t>1898 Carrolton Ave.</t>
   </si>
   <si>
-    <t>112-345-8769</t>
+    <t>345-8769</t>
+  </si>
+  <si>
+    <t>#512568</t>
+  </si>
+  <si>
+    <t>Sucess</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -442,54 +448,95 @@
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -510,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor tweaking to some .xaml files
</commit_message>
<xml_diff>
--- a/Project2/Orders.xlsx
+++ b/Project2/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21BE94B-C16F-461F-92D1-EE6F9204A9D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C0C2E5-3FBA-4E45-A7C1-329D9792E913}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Product</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Laughing Lumberjack Lager</t>
   </si>
   <si>
-    <t>Ipoh Coff</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -94,10 +91,10 @@
     <t>345-8769</t>
   </si>
   <si>
-    <t>#512568</t>
-  </si>
-  <si>
     <t>Sucess</t>
+  </si>
+  <si>
+    <t>#512825</t>
   </si>
 </sst>
 </file>
@@ -419,7 +416,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,7 +449,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -466,7 +463,7 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -480,7 +477,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -494,7 +491,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -508,7 +505,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -522,7 +519,7 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -536,16 +533,11 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -573,33 +565,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>75001</v>
@@ -608,7 +600,7 @@
         <v>812</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>